<commit_message>
Add changes to get matching working.
</commit_message>
<xml_diff>
--- a/seed/data_importer/tests/data/example-data-properties-duplicates.xlsx
+++ b/seed/data_importer/tests/data/example-data-properties-duplicates.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="42">
   <si>
     <t>50 Willow Ave SE</t>
   </si>
@@ -332,7 +332,27 @@
     <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -715,8 +735,8 @@
   </sheetPr>
   <dimension ref="A1:T14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -827,9 +847,7 @@
       <c r="L2" s="5">
         <v>42369</v>
       </c>
-      <c r="M2" s="9">
-        <v>12555</v>
-      </c>
+      <c r="M2" s="9"/>
       <c r="N2" s="9" t="s">
         <v>28</v>
       </c>
@@ -882,9 +900,7 @@
       <c r="L3" s="5">
         <v>42369</v>
       </c>
-      <c r="M3" s="9">
-        <v>12555</v>
-      </c>
+      <c r="M3" s="9"/>
       <c r="N3" s="9" t="s">
         <v>28</v>
       </c>
@@ -991,9 +1007,7 @@
       <c r="L5" s="5">
         <v>42369</v>
       </c>
-      <c r="M5" s="9">
-        <v>12555</v>
-      </c>
+      <c r="M5" s="9"/>
       <c r="N5" s="9" t="s">
         <v>28</v>
       </c>
@@ -1100,9 +1114,7 @@
       <c r="L7" s="5">
         <v>42369</v>
       </c>
-      <c r="M7" s="9">
-        <v>12555</v>
-      </c>
+      <c r="M7" s="9"/>
       <c r="N7" s="9" t="s">
         <v>28</v>
       </c>
@@ -1155,9 +1167,7 @@
       <c r="L8" s="5">
         <v>42369</v>
       </c>
-      <c r="M8" s="9">
-        <v>12555</v>
-      </c>
+      <c r="M8" s="9"/>
       <c r="N8" s="9" t="s">
         <v>28</v>
       </c>
@@ -1210,9 +1220,7 @@
       <c r="L9" s="5">
         <v>42369</v>
       </c>
-      <c r="M9" s="9">
-        <v>12555</v>
-      </c>
+      <c r="M9" s="9"/>
       <c r="N9" s="9" t="s">
         <v>28</v>
       </c>
@@ -1233,25 +1241,58 @@
       </c>
       <c r="T9" s="4"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+    <row r="10" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>22</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2264</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="4"/>
+      <c r="K10" s="3">
+        <v>125</v>
+      </c>
+      <c r="L10" s="5">
+        <v>42369</v>
+      </c>
+      <c r="M10" s="9">
+        <v>12555</v>
+      </c>
+      <c r="N10" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="R10" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="S10" s="4">
+        <v>1</v>
+      </c>
+      <c r="T10" s="4"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
@@ -1333,29 +1374,32 @@
   <sortState ref="D2:IW1452">
     <sortCondition ref="D2:D1452"/>
   </sortState>
-  <conditionalFormatting sqref="F4 D2:F2 D10 D12 F10:F14 F6">
-    <cfRule type="duplicateValues" dxfId="7" priority="102"/>
+  <conditionalFormatting sqref="F4 D2:F2 D12 F11:F14 F6">
+    <cfRule type="duplicateValues" dxfId="9" priority="103"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11 D13">
-    <cfRule type="duplicateValues" dxfId="6" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:F3">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:F5">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:F7">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:F8">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9:F9">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10:F10">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
normalize the lot_number as well. update tests
</commit_message>
<xml_diff>
--- a/seed/data_importer/tests/data/example-data-properties-duplicates.xlsx
+++ b/seed/data_importer/tests/data/example-data-properties-duplicates.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26812"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naddy/Source/LBL/seed/seed/data_importer/tests/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="151"/>
+    <workbookView xWindow="0" yWindow="8700" windowWidth="28800" windowHeight="8720" tabRatio="151"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -24,35 +19,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="43">
   <si>
     <t>50 Willow Ave SE</t>
   </si>
   <si>
-    <t>energy_score</t>
-  </si>
-  <si>
-    <t>site_eui</t>
-  </si>
-  <si>
-    <t>year_ending</t>
-  </si>
-  <si>
-    <t>property_notes</t>
-  </si>
-  <si>
-    <t>gross_floor_area</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
-    <t>address_line_1</t>
-  </si>
-  <si>
-    <t>jurisdiction_property_identifier</t>
-  </si>
-  <si>
     <t>Case A-1: 1 Property, 1 Tax Lot</t>
   </si>
   <si>
@@ -62,15 +36,9 @@
     <t>2660 Welstone Ave NE</t>
   </si>
   <si>
-    <t>property_name</t>
-  </si>
-  <si>
     <t>Hilltop Offices</t>
   </si>
   <si>
-    <t>use_description</t>
-  </si>
-  <si>
     <t>Multifamily Housing</t>
   </si>
   <si>
@@ -95,12 +63,6 @@
     <t>owner</t>
   </si>
   <si>
-    <t>owner_email</t>
-  </si>
-  <si>
-    <t>owner_telephone</t>
-  </si>
-  <si>
     <t>213-852-1238</t>
   </si>
   <si>
@@ -128,15 +90,6 @@
     <t>Rust</t>
   </si>
   <si>
-    <t>pm_parent_property_id</t>
-  </si>
-  <si>
-    <t>extra_data_1</t>
-  </si>
-  <si>
-    <t>extra_data_2</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
@@ -146,10 +99,55 @@
     <t>c</t>
   </si>
   <si>
-    <t>pm_property_id</t>
-  </si>
-  <si>
-    <t>custom_id_1</t>
+    <t>custom id 1</t>
+  </si>
+  <si>
+    <t>pm property id</t>
+  </si>
+  <si>
+    <t>pm parent propery id</t>
+  </si>
+  <si>
+    <t>property name</t>
+  </si>
+  <si>
+    <t>address line 1</t>
+  </si>
+  <si>
+    <t>use description</t>
+  </si>
+  <si>
+    <t>site eui</t>
+  </si>
+  <si>
+    <t>year ending</t>
+  </si>
+  <si>
+    <t>owner email</t>
+  </si>
+  <si>
+    <t>owner telephone</t>
+  </si>
+  <si>
+    <t>property notes</t>
+  </si>
+  <si>
+    <t>extra data 1</t>
+  </si>
+  <si>
+    <t>extra data 2</t>
+  </si>
+  <si>
+    <t>jurisdiction property identifier</t>
+  </si>
+  <si>
+    <t>gross floor area</t>
+  </si>
+  <si>
+    <t>energy score</t>
+  </si>
+  <si>
+    <t>old_jurisdiction_tax_lot</t>
   </si>
 </sst>
 </file>
@@ -157,8 +155,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -223,9 +221,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="36">
+  <cellStyleXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -261,7 +261,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -274,27 +274,33 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="36">
+  <cellStyles count="38">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -313,6 +319,7 @@
     <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -330,19 +337,10 @@
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -733,13 +731,13 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T14"/>
+  <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="1"/>
     <col min="2" max="3" width="21.5" customWidth="1"/>
@@ -747,75 +745,79 @@
     <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.83203125" customWidth="1"/>
-    <col min="9" max="9" width="19.83203125" customWidth="1"/>
-    <col min="10" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.1640625" customWidth="1"/>
-    <col min="13" max="13" width="11.83203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="13.5" style="8" customWidth="1"/>
-    <col min="17" max="17" width="39" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.83203125" customWidth="1"/>
+    <col min="11" max="12" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.1640625" customWidth="1"/>
+    <col min="14" max="14" width="11.83203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="13.5" style="6" customWidth="1"/>
+    <col min="18" max="18" width="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="10" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="10" t="s">
+    <row r="1" spans="1:21" s="8" customFormat="1" ht="12">
+      <c r="A1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="L1" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="O1" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>4</v>
+      <c r="Q1" s="15" t="s">
+        <v>35</v>
       </c>
       <c r="R1" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="S1" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="14"/>
+      <c r="S1" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="T1" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="U1" s="12"/>
     </row>
-    <row r="2" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="1" customFormat="1">
       <c r="A2" s="1">
         <v>22</v>
       </c>
@@ -827,48 +829,49 @@
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="3">
+        <v>22</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="3">
         <v>75</v>
       </c>
-      <c r="K2" s="3">
+      <c r="L2" s="3">
         <v>125</v>
       </c>
-      <c r="L2" s="5">
+      <c r="M2" s="5">
         <v>42369</v>
       </c>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="P2" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="R2" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="S2" s="4">
-        <v>1</v>
-      </c>
-      <c r="T2" s="4"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="T2" s="4">
+        <v>1</v>
+      </c>
+      <c r="U2" s="4"/>
     </row>
-    <row r="3" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" s="1" customFormat="1">
       <c r="A3" s="1">
         <v>22</v>
       </c>
@@ -880,48 +883,49 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="3">
+        <v>22</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="3">
         <v>75</v>
       </c>
-      <c r="K3" s="3">
+      <c r="L3" s="3">
         <v>125</v>
       </c>
-      <c r="L3" s="5">
+      <c r="M3" s="5">
         <v>42369</v>
       </c>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="P3" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="R3" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="S3" s="4">
-        <v>1</v>
-      </c>
-      <c r="T3" s="4"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="T3" s="4">
+        <v>1</v>
+      </c>
+      <c r="U3" s="4"/>
     </row>
-    <row r="4" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" s="1" customFormat="1">
       <c r="A4" s="1">
         <v>31</v>
       </c>
@@ -932,50 +936,51 @@
         <v>3020139</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="3">
+        <v>1</v>
+      </c>
+      <c r="L4" s="3">
+        <v>652.29999999999995</v>
+      </c>
+      <c r="M4" s="5">
+        <v>42369</v>
+      </c>
+      <c r="N4" s="7">
+        <v>513852</v>
+      </c>
+      <c r="O4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="P4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="R4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="3">
-        <v>1</v>
-      </c>
-      <c r="K4" s="3">
-        <v>652.29999999999995</v>
-      </c>
-      <c r="L4" s="5">
-        <v>42369</v>
-      </c>
-      <c r="M4" s="9">
-        <v>513852</v>
-      </c>
-      <c r="N4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="P4" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="R4" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="S4" s="4">
+      <c r="S4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="T4" s="4">
         <v>2</v>
       </c>
-      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
     </row>
-    <row r="5" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" s="1" customFormat="1">
       <c r="A5" s="1">
         <v>22</v>
       </c>
@@ -987,48 +992,49 @@
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="3">
+        <v>22</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="3">
         <v>75</v>
       </c>
-      <c r="K5" s="3">
+      <c r="L5" s="3">
         <v>125</v>
       </c>
-      <c r="L5" s="5">
+      <c r="M5" s="5">
         <v>42369</v>
       </c>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="P5" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="R5" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="S5" s="4">
-        <v>1</v>
-      </c>
-      <c r="T5" s="4"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="S5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="T5" s="4">
+        <v>1</v>
+      </c>
+      <c r="U5" s="4"/>
     </row>
-    <row r="6" spans="1:20" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" s="1" customFormat="1" ht="24" customHeight="1">
       <c r="A6" s="1">
         <v>32</v>
       </c>
@@ -1039,50 +1045,51 @@
         <v>4828379</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L6" s="5">
+        <v>12</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M6" s="5">
         <v>42369</v>
       </c>
-      <c r="M6" s="9">
+      <c r="N6" s="7">
         <v>55121</v>
       </c>
-      <c r="N6" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="P6" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="R6" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="S6" s="4">
+      <c r="O6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="S6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="T6" s="4">
         <v>3</v>
       </c>
-      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
     </row>
-    <row r="7" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" s="1" customFormat="1">
       <c r="A7" s="1">
         <v>22</v>
       </c>
@@ -1094,48 +1101,49 @@
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>0</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" s="3">
+        <v>22</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7" s="3">
         <v>75</v>
       </c>
-      <c r="K7" s="3">
+      <c r="L7" s="3">
         <v>125</v>
       </c>
-      <c r="L7" s="5">
+      <c r="M7" s="5">
         <v>42369</v>
       </c>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="P7" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="R7" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="S7" s="4">
-        <v>1</v>
-      </c>
-      <c r="T7" s="4"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="S7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="T7" s="4">
+        <v>1</v>
+      </c>
+      <c r="U7" s="4"/>
     </row>
-    <row r="8" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" s="1" customFormat="1">
       <c r="A8" s="1">
         <v>22</v>
       </c>
@@ -1147,48 +1155,49 @@
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>0</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J8" s="3">
+        <v>22</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K8" s="3">
         <v>75</v>
       </c>
-      <c r="K8" s="3">
+      <c r="L8" s="3">
         <v>125</v>
       </c>
-      <c r="L8" s="5">
+      <c r="M8" s="5">
         <v>42369</v>
       </c>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="P8" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="R8" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="S8" s="4">
-        <v>1</v>
-      </c>
-      <c r="T8" s="4"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="S8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="T8" s="4">
+        <v>1</v>
+      </c>
+      <c r="U8" s="4"/>
     </row>
-    <row r="9" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" s="1" customFormat="1">
       <c r="A9" s="1">
         <v>22</v>
       </c>
@@ -1200,48 +1209,49 @@
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>0</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9" s="3">
+        <v>22</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K9" s="3">
         <v>75</v>
       </c>
-      <c r="K9" s="3">
+      <c r="L9" s="3">
         <v>125</v>
       </c>
-      <c r="L9" s="5">
+      <c r="M9" s="5">
         <v>42369</v>
       </c>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="P9" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="R9" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="S9" s="4">
-        <v>1</v>
-      </c>
-      <c r="T9" s="4"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="S9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="T9" s="4">
+        <v>1</v>
+      </c>
+      <c r="U9" s="4"/>
     </row>
-    <row r="10" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" s="1" customFormat="1">
       <c r="A10" s="1">
         <v>22</v>
       </c>
@@ -1253,48 +1263,49 @@
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>0</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3">
+        <v>22</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3">
         <v>125</v>
       </c>
-      <c r="L10" s="5">
+      <c r="M10" s="5">
         <v>42369</v>
       </c>
-      <c r="M10" s="9">
+      <c r="N10" s="7">
         <v>12555</v>
       </c>
-      <c r="N10" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="P10" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="R10" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="S10" s="4">
-        <v>1</v>
-      </c>
-      <c r="T10" s="4"/>
+      <c r="O10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="R10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="S10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="T10" s="4">
+        <v>1</v>
+      </c>
+      <c r="U10" s="4"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="2"/>
@@ -1305,16 +1316,17 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="9"/>
-      <c r="S11" s="4"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="4"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="2"/>
@@ -1325,16 +1337,17 @@
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="11"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="4"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="4"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="2"/>
@@ -1343,18 +1356,19 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
-      <c r="J13" s="1"/>
+      <c r="J13" s="3"/>
       <c r="K13" s="1"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="9"/>
-      <c r="S13" s="4"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="4"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21">
       <c r="C14" s="1"/>
       <c r="D14" s="2"/>
       <c r="F14" s="2"/>
@@ -1363,46 +1377,52 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="13"/>
-      <c r="O14"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="9"/>
-      <c r="S14" s="4"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="11"/>
+      <c r="P14"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="4"/>
     </row>
   </sheetData>
   <sortState ref="D2:IW1452">
     <sortCondition ref="D2:D1452"/>
   </sortState>
   <conditionalFormatting sqref="F4 D2:F2 D12 F11:F14 F6">
-    <cfRule type="duplicateValues" dxfId="9" priority="103"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="103"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11 D13">
-    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:F3">
-    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:F5">
-    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:F7">
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:F8">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9:F9">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:F10">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update ubids in example files
</commit_message>
<xml_diff>
--- a/seed/data_importer/tests/data/example-data-properties-duplicates.xlsx
+++ b/seed/data_importer/tests/data/example-data-properties-duplicates.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="29005"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nlong/working/seed/seed/data_importer/tests/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="17460" tabRatio="151"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="28260" tabRatio="151"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="46">
   <si>
     <t>50 Willow Ave SE</t>
   </si>
@@ -145,6 +153,18 @@
   </si>
   <si>
     <t>old_jurisdiction_tax_lot</t>
+  </si>
+  <si>
+    <t>UBID</t>
+  </si>
+  <si>
+    <t>Z01TDR2Z+7ES-Z01TDR2Z+HX7-Z01TDR2Z+UAX</t>
+  </si>
+  <si>
+    <t>VQADDOC3+V8E-VQADDOC3+XBF-VQADDOC3+2EE</t>
+  </si>
+  <si>
+    <t>ZIUC82DT+4X5-ZIUC82DT+C4M-ZIUC82DT+YK9</t>
   </si>
 </sst>
 </file>
@@ -258,7 +278,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -296,6 +316,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="38">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -728,30 +749,36 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T14"/>
+  <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1"/>
-    <col min="2" max="3" width="21.5" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.83203125" customWidth="1"/>
-    <col min="9" max="9" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.83203125" customWidth="1"/>
-    <col min="11" max="12" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.1640625" customWidth="1"/>
-    <col min="14" max="14" width="11.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="13.5" style="6" customWidth="1"/>
-    <col min="18" max="18" width="39" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.83203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="33.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="8" customFormat="1" ht="12">
+    <row r="1" spans="1:21" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -768,50 +795,53 @@
         <v>28</v>
       </c>
       <c r="F1" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="I1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="L1" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="M1" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="N1" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="15" t="s">
+      <c r="O1" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="P1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="15" t="s">
+      <c r="Q1" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="R1" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="R1" s="14" t="s">
+      <c r="S1" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="S1" s="16" t="s">
+      <c r="T1" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="T1" s="12"/>
-    </row>
-    <row r="2" spans="1:20" s="1" customFormat="1">
+      <c r="U1" s="12"/>
+    </row>
+    <row r="2" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>22</v>
       </c>
@@ -822,47 +852,50 @@
         <v>2264</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="2" t="s">
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3" t="s">
+      <c r="I2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="3">
+      <c r="L2" s="3">
         <v>75</v>
       </c>
-      <c r="L2" s="3">
+      <c r="M2" s="3">
         <v>125</v>
       </c>
-      <c r="M2" s="5">
+      <c r="N2" s="5">
         <v>42369</v>
       </c>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7" t="s">
+      <c r="O2" s="7"/>
+      <c r="P2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="R2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="S2" s="7" t="s">
+      <c r="T2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="T2" s="4"/>
-    </row>
-    <row r="3" spans="1:20" s="1" customFormat="1">
+      <c r="U2" s="4"/>
+    </row>
+    <row r="3" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>22</v>
       </c>
@@ -873,47 +906,50 @@
         <v>2264</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="2" t="s">
+      <c r="F3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3" t="s">
+      <c r="I3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="3">
+      <c r="L3" s="3">
         <v>75</v>
       </c>
-      <c r="L3" s="3">
+      <c r="M3" s="3">
         <v>125</v>
       </c>
-      <c r="M3" s="5">
+      <c r="N3" s="5">
         <v>42369</v>
       </c>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7" t="s">
+      <c r="O3" s="7"/>
+      <c r="P3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="7" t="s">
+      <c r="R3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="S3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="S3" s="7" t="s">
+      <c r="T3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="T3" s="4"/>
-    </row>
-    <row r="4" spans="1:20" s="1" customFormat="1">
+      <c r="U3" s="4"/>
+    </row>
+    <row r="4" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>31</v>
       </c>
@@ -923,49 +959,52 @@
       <c r="D4" s="1">
         <v>3020139</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3" t="s">
+      <c r="I4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="3">
+      <c r="L4" s="3">
         <v>1</v>
       </c>
-      <c r="L4" s="3">
+      <c r="M4" s="3">
         <v>652.29999999999995</v>
       </c>
-      <c r="M4" s="5">
+      <c r="N4" s="5">
         <v>42369</v>
       </c>
-      <c r="N4" s="7">
+      <c r="O4" s="7">
         <v>513852</v>
       </c>
-      <c r="O4" s="7" t="s">
+      <c r="P4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Q4" s="7" t="s">
+      <c r="R4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="S4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="S4" s="7" t="s">
+      <c r="T4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="T4" s="4"/>
-    </row>
-    <row r="5" spans="1:20" s="1" customFormat="1">
+      <c r="U4" s="4"/>
+    </row>
+    <row r="5" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>22</v>
       </c>
@@ -976,47 +1015,50 @@
         <v>2264</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="2" t="s">
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3" t="s">
+      <c r="I5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="3">
+      <c r="L5" s="3">
         <v>75</v>
       </c>
-      <c r="L5" s="3">
+      <c r="M5" s="3">
         <v>125</v>
       </c>
-      <c r="M5" s="5">
+      <c r="N5" s="5">
         <v>42369</v>
       </c>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7" t="s">
+      <c r="O5" s="7"/>
+      <c r="P5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="Q5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Q5" s="7" t="s">
+      <c r="R5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="R5" s="4" t="s">
+      <c r="S5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="S5" s="7" t="s">
+      <c r="T5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="T5" s="4"/>
-    </row>
-    <row r="6" spans="1:20" s="1" customFormat="1" ht="24" customHeight="1">
+      <c r="U5" s="4"/>
+    </row>
+    <row r="6" spans="1:21" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>32</v>
       </c>
@@ -1026,49 +1068,52 @@
       <c r="D6" s="1">
         <v>4828379</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3" t="s">
+      <c r="I6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N6" s="5">
         <v>42369</v>
       </c>
-      <c r="N6" s="7">
+      <c r="O6" s="7">
         <v>55121</v>
       </c>
-      <c r="O6" s="7" t="s">
+      <c r="P6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="Q6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Q6" s="7" t="s">
+      <c r="R6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="R6" s="4" t="s">
+      <c r="S6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="S6" s="7" t="s">
+      <c r="T6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="T6" s="4"/>
-    </row>
-    <row r="7" spans="1:20" s="1" customFormat="1">
+      <c r="U6" s="4"/>
+    </row>
+    <row r="7" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>22</v>
       </c>
@@ -1079,47 +1124,50 @@
         <v>2264</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="2" t="s">
+      <c r="F7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3" t="s">
+      <c r="I7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="3">
+      <c r="L7" s="3">
         <v>75</v>
       </c>
-      <c r="L7" s="3">
+      <c r="M7" s="3">
         <v>125</v>
       </c>
-      <c r="M7" s="5">
+      <c r="N7" s="5">
         <v>42369</v>
       </c>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7" t="s">
+      <c r="O7" s="7"/>
+      <c r="P7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="Q7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Q7" s="7" t="s">
+      <c r="R7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="R7" s="4" t="s">
+      <c r="S7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="S7" s="7" t="s">
+      <c r="T7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="T7" s="4"/>
-    </row>
-    <row r="8" spans="1:20" s="1" customFormat="1">
+      <c r="U7" s="4"/>
+    </row>
+    <row r="8" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>22</v>
       </c>
@@ -1130,47 +1178,50 @@
         <v>2264</v>
       </c>
       <c r="E8" s="2"/>
-      <c r="F8" s="2" t="s">
+      <c r="F8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3" t="s">
+      <c r="I8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="3">
+      <c r="L8" s="3">
         <v>75</v>
       </c>
-      <c r="L8" s="3">
+      <c r="M8" s="3">
         <v>125</v>
       </c>
-      <c r="M8" s="5">
+      <c r="N8" s="5">
         <v>42369</v>
       </c>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7" t="s">
+      <c r="O8" s="7"/>
+      <c r="P8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="Q8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Q8" s="7" t="s">
+      <c r="R8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="R8" s="4" t="s">
+      <c r="S8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="S8" s="7" t="s">
+      <c r="T8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="T8" s="4"/>
-    </row>
-    <row r="9" spans="1:20" s="1" customFormat="1">
+      <c r="U8" s="4"/>
+    </row>
+    <row r="9" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>22</v>
       </c>
@@ -1181,47 +1232,50 @@
         <v>2264</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="2" t="s">
+      <c r="F9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3" t="s">
+      <c r="I9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K9" s="3">
+      <c r="L9" s="3">
         <v>75</v>
       </c>
-      <c r="L9" s="3">
+      <c r="M9" s="3">
         <v>125</v>
       </c>
-      <c r="M9" s="5">
+      <c r="N9" s="5">
         <v>42369</v>
       </c>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7" t="s">
+      <c r="O9" s="7"/>
+      <c r="P9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="Q9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Q9" s="7" t="s">
+      <c r="R9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="R9" s="4" t="s">
+      <c r="S9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="S9" s="7" t="s">
+      <c r="T9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="T9" s="4"/>
-    </row>
-    <row r="10" spans="1:20" s="1" customFormat="1">
+      <c r="U9" s="4"/>
+    </row>
+    <row r="10" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>22</v>
       </c>
@@ -1232,127 +1286,161 @@
         <v>2264</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="2" t="s">
+      <c r="F10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3" t="s">
+      <c r="I10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3">
+      <c r="L10" s="3"/>
+      <c r="M10" s="3">
         <v>125</v>
       </c>
-      <c r="M10" s="5">
+      <c r="N10" s="5">
         <v>42369</v>
       </c>
-      <c r="N10" s="7">
+      <c r="O10" s="7">
         <v>12555</v>
       </c>
-      <c r="O10" s="7" t="s">
+      <c r="P10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="P10" s="1" t="s">
+      <c r="Q10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Q10" s="7" t="s">
+      <c r="R10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="R10" s="4" t="s">
+      <c r="S10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="S10" s="7" t="s">
+      <c r="T10" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="T10" s="4"/>
-    </row>
-    <row r="11" spans="1:20">
+      <c r="U10" s="4"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="2"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="3"/>
+      <c r="F11"/>
+      <c r="G11" s="2"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="4"/>
-      <c r="S11" s="7"/>
-    </row>
-    <row r="12" spans="1:20">
+      <c r="M11" s="3"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="7"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="2"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="3"/>
+      <c r="F12"/>
+      <c r="G12" s="2"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="4"/>
-      <c r="S12" s="7"/>
-    </row>
-    <row r="13" spans="1:20">
+      <c r="M12" s="3"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="7"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="2"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="3"/>
+      <c r="F13"/>
+      <c r="G13" s="2"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
-      <c r="K13" s="1"/>
+      <c r="K13" s="3"/>
       <c r="L13" s="1"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="4"/>
-      <c r="S13" s="7"/>
-    </row>
-    <row r="14" spans="1:20">
+      <c r="M13" s="1"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="7"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C14" s="1"/>
       <c r="D14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="3"/>
+      <c r="F14"/>
+      <c r="G14" s="2"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="11"/>
-      <c r="P14"/>
-      <c r="R14" s="4"/>
-      <c r="S14" s="7"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="11"/>
+      <c r="Q14"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="7"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="F15"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="F16"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F17"/>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F18"/>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F19"/>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F20"/>
+    </row>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F21"/>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F22"/>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F23"/>
     </row>
   </sheetData>
   <sortState ref="D2:IW1452">
     <sortCondition ref="D2:D1452"/>
   </sortState>
-  <conditionalFormatting sqref="F4 D2:F2 D12 F11:F14 F6">
+  <conditionalFormatting sqref="G4 D2:E2 D12 G11:G14 G6 G2">
     <cfRule type="duplicateValues" dxfId="8" priority="103"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11 D13">
@@ -1361,31 +1449,26 @@
   <conditionalFormatting sqref="D14">
     <cfRule type="duplicateValues" dxfId="6" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:F3">
+  <conditionalFormatting sqref="D3:E3 G3">
     <cfRule type="duplicateValues" dxfId="5" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5:F5">
+  <conditionalFormatting sqref="D5:E5 G5">
     <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D7:F7">
+  <conditionalFormatting sqref="D7:E7 G7">
     <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8:F8">
+  <conditionalFormatting sqref="D8:E8 G8">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D9:F9">
+  <conditionalFormatting sqref="D9:E9 G9">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D10:F10">
+  <conditionalFormatting sqref="D10:E10 G10">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add long lat too database
</commit_message>
<xml_diff>
--- a/seed/data_importer/tests/data/example-data-properties-duplicates.xlsx
+++ b/seed/data_importer/tests/data/example-data-properties-duplicates.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="29005"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nlong/working/seed/seed/data_importer/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{69F97A56-442B-524C-AF35-1D88D5241061}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="28260" tabRatio="151"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="20480" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -170,7 +171,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -454,6 +455,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -745,17 +749,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
@@ -778,7 +782,7 @@
     <col min="20" max="20" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="8" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -841,7 +845,7 @@
       </c>
       <c r="U1" s="12"/>
     </row>
-    <row r="2" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>22</v>
       </c>
@@ -895,7 +899,7 @@
       </c>
       <c r="U2" s="4"/>
     </row>
-    <row r="3" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>22</v>
       </c>
@@ -949,7 +953,7 @@
       </c>
       <c r="U3" s="4"/>
     </row>
-    <row r="4" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>31</v>
       </c>
@@ -1004,7 +1008,7 @@
       </c>
       <c r="U4" s="4"/>
     </row>
-    <row r="5" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>22</v>
       </c>
@@ -1058,7 +1062,7 @@
       </c>
       <c r="U5" s="4"/>
     </row>
-    <row r="6" spans="1:21" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>32</v>
       </c>
@@ -1113,7 +1117,7 @@
       </c>
       <c r="U6" s="4"/>
     </row>
-    <row r="7" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>22</v>
       </c>
@@ -1167,7 +1171,7 @@
       </c>
       <c r="U7" s="4"/>
     </row>
-    <row r="8" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>22</v>
       </c>
@@ -1221,7 +1225,7 @@
       </c>
       <c r="U8" s="4"/>
     </row>
-    <row r="9" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>22</v>
       </c>
@@ -1275,7 +1279,7 @@
       </c>
       <c r="U9" s="4"/>
     </row>
-    <row r="10" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>22</v>
       </c>
@@ -1329,7 +1333,7 @@
       </c>
       <c r="U10" s="4"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="2"/>
@@ -1350,7 +1354,7 @@
       <c r="S11" s="4"/>
       <c r="T11" s="7"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="2"/>
@@ -1371,7 +1375,7 @@
       <c r="S12" s="4"/>
       <c r="T12" s="7"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="2"/>
@@ -1392,7 +1396,7 @@
       <c r="S13" s="4"/>
       <c r="T13" s="7"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C14" s="1"/>
       <c r="D14" s="2"/>
       <c r="F14"/>
@@ -1409,31 +1413,31 @@
       <c r="S14" s="4"/>
       <c r="T14" s="7"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F15"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F16"/>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="6:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F17"/>
     </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="6:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F18"/>
     </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="6:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F19"/>
     </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="6:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F20"/>
     </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="6:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F21"/>
     </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="6:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F22"/>
     </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="6:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F23"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update ubids in example file
</commit_message>
<xml_diff>
--- a/seed/data_importer/tests/data/example-data-properties-duplicates.xlsx
+++ b/seed/data_importer/tests/data/example-data-properties-duplicates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nlong/working/seed/seed/data_importer/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{69F97A56-442B-524C-AF35-1D88D5241061}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105C7342-E22B-674B-9FBD-852B50393A96}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="20480" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="440" windowWidth="25600" windowHeight="28360" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -159,13 +159,13 @@
     <t>UBID</t>
   </si>
   <si>
-    <t>Z01TDR2Z+7ES-Z01TDR2Z+HX7-Z01TDR2Z+UAX</t>
-  </si>
-  <si>
-    <t>VQADDOC3+V8E-VQADDOC3+XBF-VQADDOC3+2EE</t>
-  </si>
-  <si>
-    <t>ZIUC82DT+4X5-ZIUC82DT+C4M-ZIUC82DT+YK9</t>
+    <t>86HJQCC9+5JJ-2-3-2-3</t>
+  </si>
+  <si>
+    <t>86HJM8JW+XMV-1-4-1-3</t>
+  </si>
+  <si>
+    <t>86HJPCWJ+R59-1-5-2-4</t>
   </si>
 </sst>
 </file>
@@ -756,7 +756,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>